<commit_message>
Update to the item log
</commit_message>
<xml_diff>
--- a/documents/SB_QTI_ExampleItems.xlsx
+++ b/documents/SB_QTI_ExampleItems.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sbacdev.sharepoint.com/sites/SBMain/StudentS/Shared Documents/TIMS/QTI/QTI QC of samples (Manual)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_7CD3924FEE4196D7728725A54E3DD8A65241EE54" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4D363BC-3FDA-1545-AAD3-E584D14463E7}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="11_7CD3924FEE4196D7728725A54E3DD8A65241EE54" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{664E461D-851C-42F1-82BA-0425A95E226D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="13960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="13960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
+    <sheet name="DataDictionary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="43">
   <si>
     <t>Status</t>
   </si>
@@ -108,13 +109,64 @@
   </si>
   <si>
     <t>HTQ</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Numerical identifier of item</t>
+  </si>
+  <si>
+    <t>Numerical identifier for associated stimulus</t>
+  </si>
+  <si>
+    <t>Date item was released in QTI sample packages</t>
+  </si>
+  <si>
+    <t>ELA or Math</t>
+  </si>
+  <si>
+    <t>MC, MS, EBSR, HTQ, EQ, TI, MI, GI, SA, WER</t>
+  </si>
+  <si>
+    <t>Text to Speech</t>
+  </si>
+  <si>
+    <t>Braille file type BRF</t>
+  </si>
+  <si>
+    <t>Braile file type PRN</t>
+  </si>
+  <si>
+    <t>English glossary</t>
+  </si>
+  <si>
+    <t>American sign language</t>
+  </si>
+  <si>
+    <t>Spanish Translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translated Glossary </t>
+  </si>
+  <si>
+    <t>Illustration Glossary</t>
+  </si>
+  <si>
+    <t>Audio stimulus</t>
+  </si>
+  <si>
+    <t>Closed Captioning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +185,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -142,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,11 +219,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,6 +248,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,23 +575,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.83203125" style="1" customWidth="1"/>
-    <col min="7" max="14" width="7.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.85546875" style="1" customWidth="1"/>
+    <col min="7" max="14" width="7.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="5" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="42.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -562,7 +641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -612,7 +691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -662,7 +741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -712,7 +791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -762,7 +841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -812,7 +891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -862,7 +941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -912,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -962,7 +1041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +1101,188 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDC2AAE-0F56-437A-88D9-67DBDF01A685}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100988D3A5DB1F2074D91EDDD82E1316EE7" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b397e7678ea470e0219e6f076e5413cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15a21681-0ca0-46d2-8858-25ef113211f0" xmlns:ns3="e556f37e-2269-4362-849b-5bffb61b521a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3621bbc41f10ec74d9da89ab8237e05" ns2:_="" ns3:_="">
     <xsd:import namespace="15a21681-0ca0-46d2-8858-25ef113211f0"/>
@@ -1263,15 +1523,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1285,45 +1536,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ACBD8FA-C157-4AF9-8932-22C5231E75D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="15a21681-0ca0-46d2-8858-25ef113211f0"/>
-    <ds:schemaRef ds:uri="e556f37e-2269-4362-849b-5bffb61b521a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5FD76C0-1F2D-43F7-B2E0-5477B50702C6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5FD76C0-1F2D-43F7-B2E0-5477B50702C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ACBD8FA-C157-4AF9-8932-22C5231E75D1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF612CDE-E37B-48C3-9539-70BD10F6E5FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e556f37e-2269-4362-849b-5bffb61b521a"/>
-    <ds:schemaRef ds:uri="15a21681-0ca0-46d2-8858-25ef113211f0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF612CDE-E37B-48C3-9539-70BD10F6E5FD}"/>
 </file>
</xml_diff>